<commit_message>
replaced csv with updated one
</commit_message>
<xml_diff>
--- a/mcu_box_office.xlsx
+++ b/mcu_box_office.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27316"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="628" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C705F29-31F8-40BD-B89E-4D150E1EABDB}"/>
+  <xr:revisionPtr revIDLastSave="629" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DDD1D6A-F343-42A7-9A9E-225705D162D2}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
     <t>Tomatometer</t>
   </si>
   <si>
-    <t>Rotton Tomato Audience Score</t>
+    <t>Rotten Tomato Audience Score</t>
   </si>
   <si>
     <t>Run Time In Minutes</t>
@@ -449,7 +449,7 @@
     <tableColumn id="9" xr3:uid="{16A538B0-E6B4-477C-B393-EAFDD260DDED}" name="IMDb Score"/>
     <tableColumn id="10" xr3:uid="{57336FD3-4439-4A67-BF1D-9811E138815E}" name="Meta Score"/>
     <tableColumn id="11" xr3:uid="{106B909C-091C-46F1-92CC-7796D1F21965}" name="Tomatometer"/>
-    <tableColumn id="12" xr3:uid="{ECF61D3A-62A5-473E-ADC0-253CFACA8C89}" name="Rotton Tomato Audience Score"/>
+    <tableColumn id="12" xr3:uid="{ECF61D3A-62A5-473E-ADC0-253CFACA8C89}" name="Rotten Tomato Audience Score"/>
     <tableColumn id="13" xr3:uid="{F80CD62A-BBDD-45B0-AB71-1B3A0ECCD286}" name="Run Time In Minutes"/>
     <tableColumn id="14" xr3:uid="{C0A373D4-13F9-498B-95E4-4B7EB604F05B}" name="Phase"/>
     <tableColumn id="15" xr3:uid="{E7255CFD-5B59-4395-8E7C-98AC2F88C420}" name="Director"/>
@@ -777,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H34"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>